<commit_message>
fixed the smartmeter.js, moved data writing to the now database.js named file and fixed the calculation for Erdgas consumtion in my house. This is reflected in the global files...
</commit_message>
<xml_diff>
--- a/doc/gasVerbrauchUmrachnung.xlsx
+++ b/doc/gasVerbrauchUmrachnung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Gas Energieverrauch</t>
   </si>
@@ -46,13 +46,64 @@
   </si>
   <si>
     <t>kWh/m3</t>
+  </si>
+  <si>
+    <t>24s</t>
+  </si>
+  <si>
+    <t>=2+I/Min</t>
+  </si>
+  <si>
+    <t>=130L/h</t>
+  </si>
+  <si>
+    <t>=1,4 kW</t>
+  </si>
+  <si>
+    <t>Beispielrechnung</t>
+  </si>
+  <si>
+    <t>sekunden/Umdrehung</t>
+  </si>
+  <si>
+    <t>=s/L</t>
+  </si>
+  <si>
+    <t>L/s</t>
+  </si>
+  <si>
+    <t>L/h=</t>
+  </si>
+  <si>
+    <t>*3600</t>
+  </si>
+  <si>
+    <t>*Heizwert</t>
+  </si>
+  <si>
+    <t>/1000</t>
+  </si>
+  <si>
+    <t>=m3/h</t>
+  </si>
+  <si>
+    <t>=kW</t>
+  </si>
+  <si>
+    <t>P=E/t</t>
+  </si>
+  <si>
+    <t>L/m</t>
+  </si>
+  <si>
+    <t>1 Impuls = 0,01 Umdrehungen!!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -84,6 +135,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -102,18 +160,68 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="27">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,20 +551,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D14"/>
+  <dimension ref="A2:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:4">
+    <row r="2" spans="1:9">
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:9">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -464,16 +580,30 @@
         <f>1000/C8</f>
         <v>91.421048782271626</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="I6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="I7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -487,12 +617,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:9">
       <c r="B9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="10" spans="1:9" ht="45">
+      <c r="G10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -500,12 +635,147 @@
         <v>10.9384</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:9">
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="D14">
         <v>10.9384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="8:15">
+      <c r="H17">
+        <v>1419941870231</v>
+      </c>
+      <c r="J17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="8:15">
+      <c r="H18">
+        <v>1419941889669</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M18" t="s">
+        <v>17</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="8:15">
+      <c r="H19">
+        <v>1419941893153</v>
+      </c>
+      <c r="I19">
+        <f>H19-H17</f>
+        <v>22922</v>
+      </c>
+      <c r="J19">
+        <f>I19/100</f>
+        <v>229.22</v>
+      </c>
+      <c r="K19">
+        <f>1/J19</f>
+        <v>4.3626210627344909E-3</v>
+      </c>
+      <c r="L19">
+        <f>K19*60</f>
+        <v>0.26175726376406944</v>
+      </c>
+      <c r="M19">
+        <f>K19*3600</f>
+        <v>15.705435825844168</v>
+      </c>
+      <c r="N19">
+        <f>M19/1000</f>
+        <v>1.5705435825844168E-2</v>
+      </c>
+      <c r="O19">
+        <f>N19*$C$8</f>
+        <v>0.17179233923741383</v>
+      </c>
+    </row>
+    <row r="20" spans="8:15">
+      <c r="H20">
+        <v>1419941912666</v>
+      </c>
+      <c r="I20">
+        <f>H20-H18</f>
+        <v>22997</v>
+      </c>
+      <c r="J20">
+        <f>I20/100</f>
+        <v>229.97</v>
+      </c>
+      <c r="K20">
+        <f>1/J20</f>
+        <v>4.3483932686872199E-3</v>
+      </c>
+      <c r="L20">
+        <f>K20*60</f>
+        <v>0.26090359612123321</v>
+      </c>
+      <c r="M20">
+        <f>K20*3600</f>
+        <v>15.654215767273993</v>
+      </c>
+      <c r="N20">
+        <f>M20/1000</f>
+        <v>1.5654215767273993E-2</v>
+      </c>
+      <c r="O20">
+        <f>N20*$C$8</f>
+        <v>0.17123207374874985</v>
+      </c>
+    </row>
+    <row r="24" spans="8:15">
+      <c r="H24">
+        <f>2040-1660</f>
+        <v>380</v>
+      </c>
+      <c r="I24">
+        <v>4200</v>
+      </c>
+      <c r="J24">
+        <f>I24/H24</f>
+        <v>11.052631578947368</v>
+      </c>
+    </row>
+    <row r="25" spans="8:15">
+      <c r="H25">
+        <f>2050-1670</f>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="26" spans="8:15">
+      <c r="H26">
+        <v>1670</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed log status in globalParameters.json
</commit_message>
<xml_diff>
--- a/doc/gasVerbrauchUmrachnung.xlsx
+++ b/doc/gasVerbrauchUmrachnung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Gas Energieverrauch</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>1 Impuls = 0,01 Umdrehungen!!!</t>
+  </si>
+  <si>
+    <t>/Tag</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>/h</t>
+  </si>
+  <si>
+    <t>Brockdorf kW</t>
   </si>
 </sst>
 </file>
@@ -189,11 +201,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -551,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O26"/>
+  <dimension ref="A2:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -648,7 +661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="8:15">
+    <row r="17" spans="2:15">
       <c r="H17">
         <v>1419941870231</v>
       </c>
@@ -665,7 +678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="8:15">
+    <row r="18" spans="2:15">
       <c r="H18">
         <v>1419941889669</v>
       </c>
@@ -688,7 +701,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="8:15">
+    <row r="19" spans="2:15">
       <c r="H19">
         <v>1419941893153</v>
       </c>
@@ -721,7 +734,7 @@
         <v>0.17179233923741383</v>
       </c>
     </row>
-    <row r="20" spans="8:15">
+    <row r="20" spans="2:15">
       <c r="H20">
         <v>1419941912666</v>
       </c>
@@ -754,7 +767,7 @@
         <v>0.17123207374874985</v>
       </c>
     </row>
-    <row r="24" spans="8:15">
+    <row r="24" spans="2:15">
       <c r="H24">
         <f>2040-1660</f>
         <v>380</v>
@@ -767,15 +780,51 @@
         <v>11.052631578947368</v>
       </c>
     </row>
-    <row r="25" spans="8:15">
+    <row r="25" spans="2:15">
       <c r="H25">
         <f>2050-1670</f>
         <v>380</v>
       </c>
     </row>
-    <row r="26" spans="8:15">
+    <row r="26" spans="2:15">
       <c r="H26">
         <v>1670</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="B29">
+        <v>53000</v>
+      </c>
+      <c r="C29">
+        <f>B29/4</f>
+        <v>13250</v>
+      </c>
+      <c r="D29">
+        <f>C29/24</f>
+        <v>552.08333333333337</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1480000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="E30">
+        <f>E29/D29</f>
+        <v>2680.7547169811319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>